<commit_message>
delete 얀센 from 2nd dose
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05030830.xlsx
+++ b/data/vaccine/vaccination_12dose_05030830.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjlee/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FCCDC0-7106-754B-A4EE-4B22F139DA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A2EB56-0C5E-E74E-8CE5-1EF9E8DC8D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="580" windowWidth="27640" windowHeight="15300" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="19780" yWindow="3320" windowWidth="27640" windowHeight="15300" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
     <sheet name="2nd dose" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -126,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,12 +147,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -530,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="B22:C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,7 +839,7 @@
         <v>6032090</v>
       </c>
       <c r="G12" s="2">
-        <v>33118792</v>
+        <v>3318792</v>
       </c>
       <c r="H12" s="2">
         <v>1795097</v>
@@ -1043,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1188,25 +1182,32 @@
         <v>44382</v>
       </c>
       <c r="B11" s="2">
-        <v>310844</v>
+        <f>310844-17</f>
+        <v>310827</v>
       </c>
       <c r="C11" s="2">
-        <v>965064</v>
+        <f>965064-802874</f>
+        <v>162190</v>
       </c>
       <c r="D11" s="2">
-        <v>379454</v>
+        <f>379454-197434</f>
+        <v>182020</v>
       </c>
       <c r="E11" s="2">
-        <v>307143</v>
+        <f>307143-60318</f>
+        <v>246825</v>
       </c>
       <c r="F11" s="2">
-        <v>232244</v>
+        <f>232244-60206</f>
+        <v>172038</v>
       </c>
       <c r="G11" s="2">
-        <v>1454178</v>
+        <f>1454178-8270</f>
+        <v>1445908</v>
       </c>
       <c r="H11" s="2">
-        <v>1672675</v>
+        <f>1672675-320</f>
+        <v>1672355</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1214,25 +1215,32 @@
         <v>44389</v>
       </c>
       <c r="B12" s="2">
-        <v>537578</v>
+        <f>537578-18</f>
+        <v>537560</v>
       </c>
       <c r="C12" s="2">
-        <v>987723</v>
+        <f>987723-802951</f>
+        <v>184772</v>
       </c>
       <c r="D12" s="2">
-        <v>424823</v>
+        <f>424823-197528</f>
+        <v>227295</v>
       </c>
       <c r="E12" s="2">
-        <v>401269</v>
+        <f>401269-60379</f>
+        <v>340890</v>
       </c>
       <c r="F12" s="2">
-        <v>338545</v>
+        <f>338545-60218</f>
+        <v>278327</v>
       </c>
       <c r="G12" s="2">
-        <v>1485653</v>
+        <f>1485653-8272</f>
+        <v>1477381</v>
       </c>
       <c r="H12" s="2">
-        <v>1697818</v>
+        <f>1697818-320</f>
+        <v>1697498</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1240,25 +1248,32 @@
         <v>44396</v>
       </c>
       <c r="B13" s="2">
-        <v>742006</v>
+        <f>742006-18</f>
+        <v>741988</v>
       </c>
       <c r="C13" s="2">
-        <v>1075256</v>
+        <f>1075256-802956</f>
+        <v>272300</v>
       </c>
       <c r="D13" s="2">
-        <v>562643</v>
+        <f>562643-197534</f>
+        <v>365109</v>
       </c>
       <c r="E13" s="2">
-        <v>546540</v>
+        <f>546540-60381</f>
+        <v>486159</v>
       </c>
       <c r="F13" s="2">
-        <v>412978</v>
+        <f>412978-60222</f>
+        <v>352756</v>
       </c>
       <c r="G13" s="2">
-        <v>1509595</v>
+        <f>1509595-8274</f>
+        <v>1501321</v>
       </c>
       <c r="H13" s="2">
-        <v>1716454</v>
+        <f>1716454-320</f>
+        <v>1716134</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1266,32 +1281,32 @@
         <v>44403</v>
       </c>
       <c r="B14" s="3">
-        <f>754939+18</f>
-        <v>754957</v>
+        <f>754939</f>
+        <v>754939</v>
       </c>
       <c r="C14" s="3">
-        <f>335462+802959</f>
-        <v>1138421</v>
+        <f>335462</f>
+        <v>335462</v>
       </c>
       <c r="D14" s="3">
-        <f>437733+197535</f>
-        <v>635268</v>
+        <f>437733</f>
+        <v>437733</v>
       </c>
       <c r="E14" s="3">
-        <f>551208+60386</f>
-        <v>611594</v>
+        <f>551208</f>
+        <v>551208</v>
       </c>
       <c r="F14" s="3">
-        <f>387426+60227</f>
-        <v>447653</v>
+        <f>387426</f>
+        <v>387426</v>
       </c>
       <c r="G14" s="3">
-        <f>1517041+8277</f>
-        <v>1525318</v>
+        <f>1517041</f>
+        <v>1517041</v>
       </c>
       <c r="H14" s="3">
-        <f>1729588+320</f>
-        <v>1729908</v>
+        <f>1729588</f>
+        <v>1729588</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -1299,25 +1314,32 @@
         <v>44410</v>
       </c>
       <c r="B15" s="2">
-        <v>854927</v>
+        <f>854927-18</f>
+        <v>854909</v>
       </c>
       <c r="C15" s="2">
-        <v>1165851</v>
+        <f>1165851-802983</f>
+        <v>362868</v>
       </c>
       <c r="D15" s="2">
-        <v>662120</v>
+        <f>662120-197544</f>
+        <v>464576</v>
       </c>
       <c r="E15" s="2">
-        <v>632641</v>
+        <f>632641-60393</f>
+        <v>572248</v>
       </c>
       <c r="F15" s="2">
-        <v>543993</v>
+        <f>543993-60227</f>
+        <v>483766</v>
       </c>
       <c r="G15" s="2">
-        <v>1548144</v>
+        <f>1548144-8276</f>
+        <v>1539868</v>
       </c>
       <c r="H15" s="2">
-        <v>1738733</v>
+        <f>1738733-321</f>
+        <v>1738412</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
@@ -1325,32 +1347,32 @@
         <v>44417</v>
       </c>
       <c r="B16" s="3">
-        <f>883966+18</f>
-        <v>883984</v>
+        <f>883966</f>
+        <v>883966</v>
       </c>
       <c r="C16" s="3">
-        <f>454249+802982</f>
-        <v>1257231</v>
+        <f>454249</f>
+        <v>454249</v>
       </c>
       <c r="D16" s="3">
-        <f>641635+197547</f>
-        <v>839182</v>
+        <f>641635</f>
+        <v>641635</v>
       </c>
       <c r="E16" s="3">
-        <f>693297+60393</f>
-        <v>753690</v>
+        <f>693297</f>
+        <v>693297</v>
       </c>
       <c r="F16" s="3">
-        <f>545683+60231</f>
-        <v>605914</v>
+        <f>545683</f>
+        <v>545683</v>
       </c>
       <c r="G16" s="3">
-        <f>1558023+8277</f>
-        <v>1566300</v>
+        <f>1558023</f>
+        <v>1558023</v>
       </c>
       <c r="H16" s="3">
-        <f>1750721+321</f>
-        <v>1751042</v>
+        <f>1750721</f>
+        <v>1750721</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1358,25 +1380,32 @@
         <v>44424</v>
       </c>
       <c r="B17" s="2">
-        <v>1379694</v>
+        <f>1379694-18</f>
+        <v>1379676</v>
       </c>
       <c r="C17" s="2">
-        <v>1376128</v>
+        <f>1376128-802987</f>
+        <v>573141</v>
       </c>
       <c r="D17" s="2">
-        <v>1029639</v>
+        <f>1029639-197547</f>
+        <v>832092</v>
       </c>
       <c r="E17" s="2">
-        <v>926979</v>
+        <f>926979-60395</f>
+        <v>866584</v>
       </c>
       <c r="F17" s="2">
-        <v>1119437</v>
+        <f>1119437-60231</f>
+        <v>1059206</v>
       </c>
       <c r="G17" s="2">
-        <v>2148619</v>
+        <f>2148619-8278</f>
+        <v>2140341</v>
       </c>
       <c r="H17" s="2">
-        <v>1760759</v>
+        <f>1760759-321</f>
+        <v>1760438</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1384,25 +1413,32 @@
         <v>44431</v>
       </c>
       <c r="B18" s="3">
-        <v>1445177</v>
+        <f>1445177-19</f>
+        <v>1445158</v>
       </c>
       <c r="C18" s="2">
-        <v>1428880</v>
+        <f>1428880-802987</f>
+        <v>625893</v>
       </c>
       <c r="D18" s="2">
-        <v>1178430</v>
+        <f>1178430-197549</f>
+        <v>980881</v>
       </c>
       <c r="E18" s="2">
-        <v>1080805</v>
+        <f>1080805-60396</f>
+        <v>1020409</v>
       </c>
       <c r="F18" s="2">
-        <v>1970186</v>
+        <f>1970186-60234</f>
+        <v>1909952</v>
       </c>
       <c r="G18" s="2">
-        <v>2683749</v>
+        <f>2683749-8278</f>
+        <v>2675471</v>
       </c>
       <c r="H18" s="2">
-        <v>1765298</v>
+        <f>1765298-321</f>
+        <v>1764977</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1410,25 +1446,32 @@
         <v>44438</v>
       </c>
       <c r="B19" s="3">
-        <v>1465804</v>
+        <f>1465804-22</f>
+        <v>1465782</v>
       </c>
       <c r="C19" s="2">
-        <v>1522510</v>
+        <f>1522510-824599</f>
+        <v>697911</v>
       </c>
       <c r="D19" s="2">
-        <v>1362553</v>
+        <f>1362553-218975</f>
+        <v>1143578</v>
       </c>
       <c r="E19" s="2">
-        <v>1237519</v>
+        <f>1237519-65430</f>
+        <v>1172089</v>
       </c>
       <c r="F19" s="2">
-        <v>4246240</v>
+        <f>4246240-61377</f>
+        <v>4184863</v>
       </c>
       <c r="G19" s="2">
-        <v>2999176</v>
+        <f>2999176-8461</f>
+        <v>2990715</v>
       </c>
       <c r="H19" s="2">
-        <v>1772218</v>
+        <f>1772218-557</f>
+        <v>1771661</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update vaccine dose by age
</commit_message>
<xml_diff>
--- a/data/vaccine/vaccination_12dose_05030830.xlsx
+++ b/data/vaccine/vaccination_12dose_05030830.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\JJ_YJ shared folder\data\for code\vaccine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iyunjeong/repos/COVID19_SeoulGyeonggi/data/vaccine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07999496-F077-40F6-A151-3BE4B279E268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED47697-C1DF-8D4C-90A7-EEC3CF66D908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="15310" windowHeight="7360" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
+    <workbookView xWindow="15440" yWindow="2460" windowWidth="21300" windowHeight="13680" activeTab="1" xr2:uid="{0BC8E184-C19A-CB40-8BBD-2FB6EDF0175E}"/>
   </bookViews>
   <sheets>
     <sheet name="1st dose" sheetId="1" r:id="rId1"/>
@@ -43,18 +43,18 @@
   <commentList>
     <comment ref="B18" authorId="0" shapeId="0" xr:uid="{3FF07971-2D00-ED44-BF97-BB699E7DCC05}">
       <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     12-17세: 15,273
 미포함</t>
       </text>
     </comment>
     <comment ref="B19" authorId="1" shapeId="0" xr:uid="{2856A7CE-C2DA-CA4E-949B-DC7D60C647FD}">
       <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     12-17세: 15,287
 미포함</t>
       </text>
@@ -72,18 +72,18 @@
   <commentList>
     <comment ref="B18" authorId="0" shapeId="0" xr:uid="{41A9A404-812B-1E40-BB1C-C84BAA7CD657}">
       <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     12-17세: 12,596
 미포함</t>
       </text>
     </comment>
     <comment ref="B19" authorId="1" shapeId="0" xr:uid="{A23C0DDA-6719-444D-8906-8FF74C63C4D8}">
       <text>
-        <t>[스레드 댓글]
-사용 중인 버전의 Excel에서 이 스레드 댓글을 읽을 수 있지만 파일을 이후 버전의 Excel에서 열면 편집 내용이 모두 제거됩니다. 자세한 정보: https://go.microsoft.com/fwlink/?linkid=870924.
-댓글:
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
     12-17세: 13,051
 미포함</t>
       </text>
@@ -124,33 +124,33 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -175,17 +175,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -529,18 +529,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2E4180-383F-D540-B7B7-6029C29EA127}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44319</v>
       </c>
@@ -592,7 +592,7 @@
         <v>1053621</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44326</v>
       </c>
@@ -618,7 +618,7 @@
         <v>1108728</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44333</v>
       </c>
@@ -644,7 +644,7 @@
         <v>1124225</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44340</v>
       </c>
@@ -670,7 +670,7 @@
         <v>1149494</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44347</v>
       </c>
@@ -696,7 +696,7 @@
         <v>1352586</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44354</v>
       </c>
@@ -722,7 +722,7 @@
         <v>1552002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44361</v>
       </c>
@@ -748,7 +748,7 @@
         <v>1738183</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44368</v>
       </c>
@@ -774,7 +774,7 @@
         <v>1758341</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44375</v>
       </c>
@@ -800,7 +800,7 @@
         <v>1774711</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44382</v>
       </c>
@@ -826,7 +826,7 @@
         <v>1787068</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44389</v>
       </c>
@@ -852,7 +852,7 @@
         <v>1795097</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44396</v>
       </c>
@@ -878,7 +878,7 @@
         <v>1805666</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44403</v>
       </c>
@@ -904,7 +904,7 @@
         <v>1810437</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44410</v>
       </c>
@@ -930,7 +930,7 @@
         <v>1815054</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44417</v>
       </c>
@@ -956,7 +956,7 @@
         <v>1823689</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44424</v>
       </c>
@@ -982,7 +982,7 @@
         <v>1835569</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44431</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>1846122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44438</v>
       </c>
@@ -1032,6 +1032,58 @@
       </c>
       <c r="H19" s="2">
         <v>1855490</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44445</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3497433</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3091102</v>
+      </c>
+      <c r="D20" s="2">
+        <v>3563988</v>
+      </c>
+      <c r="E20" s="2">
+        <v>7843679</v>
+      </c>
+      <c r="F20" s="2">
+        <v>6656881</v>
+      </c>
+      <c r="G20" s="2">
+        <v>3474049</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1863037</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B21" s="2">
+        <v>4459494</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3912573</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4845871</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7895083</v>
+      </c>
+      <c r="F21" s="2">
+        <v>6677000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3480174</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1867227</v>
       </c>
     </row>
   </sheetData>
@@ -1043,15 +1095,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA06488B-6AE1-6D45-B18E-AB20070D0C15}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="17.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +1132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44319</v>
       </c>
@@ -1089,7 +1144,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44326</v>
       </c>
@@ -1101,7 +1156,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44333</v>
       </c>
@@ -1113,7 +1168,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44340</v>
       </c>
@@ -1125,7 +1180,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44347</v>
       </c>
@@ -1137,7 +1192,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44354</v>
       </c>
@@ -1149,7 +1204,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44361</v>
       </c>
@@ -1161,7 +1216,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44368</v>
       </c>
@@ -1173,7 +1228,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>44375</v>
       </c>
@@ -1185,7 +1240,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>44382</v>
       </c>
@@ -1218,7 +1273,7 @@
         <v>1672355</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>44389</v>
       </c>
@@ -1251,7 +1306,7 @@
         <v>1697498</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>44396</v>
       </c>
@@ -1284,7 +1339,7 @@
         <v>1716134</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>44403</v>
       </c>
@@ -1317,7 +1372,7 @@
         <v>1729588</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44410</v>
       </c>
@@ -1350,7 +1405,7 @@
         <v>1738412</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>44417</v>
       </c>
@@ -1383,7 +1438,7 @@
         <v>1750721</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>44424</v>
       </c>
@@ -1416,7 +1471,7 @@
         <v>1760438</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>44431</v>
       </c>
@@ -1449,7 +1504,7 @@
         <v>1764977</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>44438</v>
       </c>
@@ -1480,6 +1535,72 @@
       <c r="H19" s="2">
         <f>1772218-557</f>
         <v>1771661</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44445</v>
+      </c>
+      <c r="B20" s="2">
+        <f>1584973-43</f>
+        <v>1584930</v>
+      </c>
+      <c r="C20" s="2">
+        <f>1772048-860571</f>
+        <v>911477</v>
+      </c>
+      <c r="D20" s="2">
+        <f>1709079-251759</f>
+        <v>1457320</v>
+      </c>
+      <c r="E20" s="2">
+        <f>1542659-80621</f>
+        <v>1462038</v>
+      </c>
+      <c r="F20" s="2">
+        <f>6040407-65402</f>
+        <v>5975005</v>
+      </c>
+      <c r="G20" s="2">
+        <f>3309226-9060</f>
+        <v>3300166</v>
+      </c>
+      <c r="H20" s="2">
+        <f>1780185-1134</f>
+        <v>1779051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>44452</v>
+      </c>
+      <c r="B21" s="2">
+        <f>1912209-66</f>
+        <v>1912143</v>
+      </c>
+      <c r="C21" s="2">
+        <f>2011816-887563</f>
+        <v>1124253</v>
+      </c>
+      <c r="D21" s="2">
+        <f>2014986-276082</f>
+        <v>1738904</v>
+      </c>
+      <c r="E21" s="2">
+        <f>2814585-93245</f>
+        <v>2721340</v>
+      </c>
+      <c r="F21" s="2">
+        <f>6167274-68803</f>
+        <v>6098471</v>
+      </c>
+      <c r="G21" s="2">
+        <f>3338637-9616</f>
+        <v>3329021</v>
+      </c>
+      <c r="H21" s="2">
+        <f>1787410-1486</f>
+        <v>1785924</v>
       </c>
     </row>
   </sheetData>

</xml_diff>